<commit_message>
Added Unit and Weapon objects
</commit_message>
<xml_diff>
--- a/Fate1/bin/Debug/net6.0/Ironjaws.xlsx
+++ b/Fate1/bin/Debug/net6.0/Ironjaws.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tough\OneDrive\Desktop\Programming\FateWeaver\Fate1\bin\Debug\net6.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4C48D9-7927-459F-9C46-E58AC851F648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9305153-A64E-446A-9F80-862D77632FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A301D7C7-C306-4AEB-A9A6-66C0DD57AEAC}"/>
+    <workbookView xWindow="4980" yWindow="2952" windowWidth="17280" windowHeight="8964" xr2:uid="{A301D7C7-C306-4AEB-A9A6-66C0DD57AEAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -177,10 +177,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -203,13 +211,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -522,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A50461-1793-4406-8194-B73B9E572950}">
-  <dimension ref="A1:AH4"/>
+  <dimension ref="A1:BO4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -556,7 +567,7 @@
     <col min="34" max="34" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -660,7 +671,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -739,8 +750,9 @@
       <c r="Z2">
         <v>1</v>
       </c>
+      <c r="BO2" s="1"/>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -796,7 +808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
Added calculations for percentage kill
</commit_message>
<xml_diff>
--- a/Fate1/bin/Debug/net6.0/Ironjaws.xlsx
+++ b/Fate1/bin/Debug/net6.0/Ironjaws.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tough\OneDrive\Desktop\Programming\FateWeaver\Fate1\bin\Debug\net6.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0c96b76f67de85b5/Desktop/Programming/FateWeaver/Fate1/bin/Debug/net6.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9305153-A64E-446A-9F80-862D77632FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{F3620AAC-583B-41CC-A193-9FBBFF41F4AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{612CB56E-615A-4357-9C5B-CD0BE56952AA}"/>
   <bookViews>
-    <workbookView xWindow="4980" yWindow="2952" windowWidth="17280" windowHeight="8964" xr2:uid="{A301D7C7-C306-4AEB-A9A6-66C0DD57AEAC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A301D7C7-C306-4AEB-A9A6-66C0DD57AEAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -234,6 +234,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -525,7 +529,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -536,7 +540,7 @@
   <dimension ref="A1:BO4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
wait does it work??
</commit_message>
<xml_diff>
--- a/Fate1/bin/Debug/net6.0/Ironjaws.xlsx
+++ b/Fate1/bin/Debug/net6.0/Ironjaws.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tough\OneDrive\Desktop\Programming\FateWeaver\Fate1\bin\Debug\net6.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OtherProgram\FateWeaver\Fate1\bin\Debug\net6.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF134810-A2F9-4230-BE88-341A6F961BF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35050919-D31C-4AD1-9466-7F77C9994501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A301D7C7-C306-4AEB-A9A6-66C0DD57AEAC}"/>
   </bookViews>
@@ -547,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A50461-1793-4406-8194-B73B9E572950}">
   <dimension ref="A1:BO5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>